<commit_message>
add score, and restart add all the body
</commit_message>
<xml_diff>
--- a/flags.xlsx
+++ b/flags.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\sex_party\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE56A4E5-0ACA-426B-A261-D59BFA776283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE23D953-9AC5-4804-A7DA-C4C478C7BBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="13">
   <si>
     <t>light_purple</t>
   </si>
@@ -86,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +165,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD8603"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -202,6 +214,8 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,6 +224,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFD8603"/>
       <color rgb="FFA139BD"/>
       <color rgb="FF9936B4"/>
       <color rgb="FF8439BD"/>
@@ -219,7 +234,6 @@
       <color rgb="FFFF5050"/>
       <color rgb="FF009999"/>
       <color rgb="FF00FFCC"/>
-      <color rgb="FFAC58A0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1154,7 +1168,7 @@
   <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="12"/>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="24" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="22" t="s">
@@ -1268,7 +1282,7 @@
       <c r="K4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="8" t="s">
@@ -1486,21 +1500,21 @@
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="C12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="10"/>
       <c r="H12" s="16" t="s">
         <v>4</v>
       </c>
+      <c r="K12" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="L12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="M12" s="12"/>
       <c r="N12" s="19" t="s">
         <v>9</v>
       </c>

</xml_diff>